<commit_message>
Cleaned up a bit. User can now enter filename.
</commit_message>
<xml_diff>
--- a/Demo.xlsx
+++ b/Demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert\Documents\Github\ExcelToText\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F987A831-6735-4195-A801-AE7C9312D737}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD42350-5BCE-49B1-B5E9-B4AE65A4E5B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30345" yWindow="960" windowWidth="21600" windowHeight="11505" xr2:uid="{998E95EE-9DC3-49EA-8162-6DD55478D9AB}"/>
   </bookViews>
@@ -436,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A942864-6DB7-470A-B384-B72F92148259}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,12 +685,17 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C33" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>